<commit_message>
update pelajaran web design fundamental semester 1, pertemuan kedua
- table
- pembuatan kolom menggunakan div
- styling margin
- github
</commit_message>
<xml_diff>
--- a/Web Design Fundamental Semester 1/SampleDesign1/HTML Cheatsheet.xlsx
+++ b/Web Design Fundamental Semester 1/SampleDesign1/HTML Cheatsheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heberthendrikpelapelapon/SGU Class/sem1/Web Design Fundamental Semester 1/SampleDesign1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC8737D-9FE4-C242-9CAE-1CF13BACE005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA97E5C-A613-A040-915D-95223A6D76F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="3060" windowWidth="36320" windowHeight="17440" xr2:uid="{3D25CE0B-5C45-3947-9250-D097231F7906}"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="27720" windowHeight="17540" xr2:uid="{3D25CE0B-5C45-3947-9250-D097231F7906}"/>
   </bookViews>
   <sheets>
     <sheet name="HTML TAG" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>&lt;h1&gt;</t>
   </si>
@@ -118,6 +119,51 @@
   </si>
   <si>
     <t>Diletakan di antara &lt;head&gt;&lt;/head&gt;</t>
+  </si>
+  <si>
+    <t>Ricky</t>
+  </si>
+  <si>
+    <t>Titan</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;</t>
+  </si>
+  <si>
+    <t>Reserve display website, full, dari kiri hingga kanan website</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;</t>
+  </si>
+  <si>
+    <t>Dylan</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Reserve display website, hanya sepanjang content saja.</t>
+  </si>
+  <si>
+    <t>Keterangan: inline</t>
+  </si>
+  <si>
+    <t>&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>Untuk membuat tabel.</t>
+  </si>
+  <si>
+    <t>&lt;tr&gt;</t>
+  </si>
+  <si>
+    <t>Untuk membuat row baru dalam 1 table</t>
+  </si>
+  <si>
+    <t>&lt;td&gt;</t>
+  </si>
+  <si>
+    <t>Untuk membuat cell baru dalam 1 row di dalam 1 table</t>
   </si>
 </sst>
 </file>
@@ -642,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CABB8FA-C753-9E4A-B2D0-D6A67A19CE55}">
-  <dimension ref="B2:G16"/>
+  <dimension ref="B2:G31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C31" sqref="C4:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,6 +861,123 @@
       <c r="F16" s="13"/>
       <c r="G16" s="8"/>
     </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="9"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="7"/>
+      <c r="C19" s="13"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="9"/>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="7"/>
+      <c r="C22" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="9"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="7"/>
+      <c r="C25" s="13"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="9"/>
+      <c r="C26" s="11"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="7"/>
+      <c r="C28" s="13"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="9"/>
+      <c r="C29" s="11"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="7"/>
+      <c r="C31" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680B1F71-FE3E-AE4A-9C16-E039E57B7AA5}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>